<commit_message>
검사 성적서 value excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excelTemplate/inspection_result_template_01.xlsx
+++ b/src/main/resources/excelTemplate/inspection_result_template_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>상호</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,18 +123,6 @@
   </si>
   <si>
     <t>${info.NOTE}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>${info.PRODUCT_NUM}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>${info.POINT_POSITION}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>${info.POINT_NUM}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -153,6 +141,40 @@
   </si>
   <si>
     <t>날짜기입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${DATA.PRODUCT_NUM}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${data3}" var="DATA"&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${data2}" var="POINT"&gt;</t>
+  </si>
+  <si>
+    <t>${POINT.POINT_NUM}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${POINT.POINT_POSITION}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;jx:forEach items="${POINT.list}" var="cols"&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${cols}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;/jx:forEach&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -160,7 +182,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +249,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,8 +272,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -552,54 +589,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -607,47 +623,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -667,25 +698,52 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,55 +761,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="358140" y="2446020"/>
-          <a:ext cx="9784080" cy="7338060"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,212 +1026,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M47"/>
+  <dimension ref="B1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.69921875" style="15" customWidth="1"/>
-    <col min="2" max="8" width="10.69921875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="12.69921875" style="15" customWidth="1"/>
-    <col min="10" max="12" width="10.69921875" style="15" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="15"/>
+    <col min="1" max="1" width="4.69921875" style="5" customWidth="1"/>
+    <col min="2" max="3" width="8.69921875" style="5" customWidth="1"/>
+    <col min="4" max="8" width="10.69921875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.69921875" style="5" customWidth="1"/>
+    <col min="10" max="12" width="10.69921875" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="38" t="s">
-        <v>29</v>
+      <c r="K3" s="20"/>
+      <c r="L3" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="35" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="1" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="36"/>
     </row>
     <row r="5" spans="2:13" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="32"/>
+      <c r="F5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>31</v>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="2:13" s="2" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="2:13" s="1" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="5" t="s">
+      <c r="L7" s="42"/>
+      <c r="M7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="18" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="20" t="s">
+      <c r="L8" s="38"/>
+      <c r="M8" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="10" spans="2:13" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="40"/>
+      <c r="D10" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="26"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="46"/>
     </row>
     <row r="11" spans="2:13" ht="7.95" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="46" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="29" t="s">
-        <v>25</v>
+    <row r="45" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="2:6" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B47" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" s="14"/>
+    <row r="47" spans="2:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="F47" s="15"/>
+    </row>
+    <row r="48" spans="2:6" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="B48" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B49" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="D10:M10"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="B7:C7"/>
@@ -1237,6 +1273,5 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>